<commit_message>
estimated initial sampling time
</commit_message>
<xml_diff>
--- a/results/2013.11.25_dac_paper_params/data.xlsx
+++ b/results/2013.11.25_dac_paper_params/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="3030" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="31">
   <si>
     <t># On my Laptop Computer (DELL Latitude E6430)</t>
   </si>
@@ -98,6 +98,15 @@
   </si>
   <si>
     <t>Second Output</t>
+  </si>
+  <si>
+    <t>Static Architecture</t>
+  </si>
+  <si>
+    <t>slower than HyPER</t>
+  </si>
+  <si>
+    <t>Initial</t>
   </si>
 </sst>
 </file>
@@ -105,9 +114,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="172" formatCode="0.0E+00"/>
+    <numFmt numFmtId="164" formatCode="0.0E+00"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -250,14 +266,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -272,10 +286,10 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -288,8 +302,15 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Prozent" xfId="1" builtinId="5"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -592,10 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W36"/>
+  <dimension ref="A1:AE36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S13" sqref="S13"/>
+      <selection activeCell="AE7" sqref="AE7:AE13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -605,47 +626,56 @@
     <col min="17" max="17" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="Q3" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
-      <c r="V3" s="1"/>
-      <c r="W3" s="1"/>
-    </row>
-    <row r="4" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R3" s="29"/>
+      <c r="S3" s="29"/>
+      <c r="T3" s="29"/>
+      <c r="U3" s="29"/>
+      <c r="V3" s="29"/>
+      <c r="W3" s="29"/>
+      <c r="X3" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y3" s="29"/>
+      <c r="Z3" s="29"/>
+      <c r="AA3" s="29"/>
+    </row>
+    <row r="4" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="N4" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
+      <c r="O4" s="29"/>
+      <c r="P4" s="29"/>
       <c r="T4" t="s">
         <v>24</v>
       </c>
       <c r="V4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="AD4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="I5" t="s">
         <v>3</v>
       </c>
@@ -661,22 +691,22 @@
       <c r="M5" t="s">
         <v>26</v>
       </c>
-      <c r="N5" s="3" t="s">
+      <c r="N5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="O5" s="4" t="s">
+      <c r="O5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="P5" s="5" t="s">
+      <c r="P5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="Q5" s="3" t="s">
+      <c r="Q5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="R5" s="4" t="s">
+      <c r="R5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="S5" s="5" t="s">
+      <c r="S5" s="4" t="s">
         <v>15</v>
       </c>
       <c r="T5" t="s">
@@ -691,8 +721,23 @@
       <c r="W5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X5" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD5">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -711,22 +756,22 @@
       <c r="F6" t="s">
         <v>8</v>
       </c>
-      <c r="N6" s="6" t="s">
+      <c r="N6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="O6" s="7" t="s">
+      <c r="O6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="P6" s="8" t="s">
+      <c r="P6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="Q6" s="6" t="s">
+      <c r="Q6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="R6" s="7" t="s">
+      <c r="R6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="S6" s="8" t="s">
+      <c r="S6" s="7" t="s">
         <v>14</v>
       </c>
       <c r="T6" t="s">
@@ -735,8 +780,20 @@
       <c r="U6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X6" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0</v>
       </c>
@@ -762,41 +819,41 @@
         <f>B7</f>
         <v>4</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K7" s="1">
         <f>C13</f>
         <v>72504205</v>
       </c>
-      <c r="L7" s="14">
+      <c r="L7" s="13">
         <f>K7*J7</f>
         <v>290016820</v>
       </c>
-      <c r="M7" s="13">
+      <c r="M7" s="12">
         <f>K7</f>
         <v>72504205</v>
       </c>
-      <c r="N7" s="22">
+      <c r="N7" s="21">
         <v>2.8594900000000001</v>
       </c>
-      <c r="O7" s="7">
+      <c r="O7" s="6">
         <v>30.6</v>
       </c>
-      <c r="P7" s="18">
+      <c r="P7" s="17">
         <f t="shared" ref="P7:P10" si="0">N7*O7</f>
         <v>87.500394</v>
       </c>
-      <c r="Q7" s="22">
+      <c r="Q7" s="21">
         <f>L7/T7</f>
         <v>0.58003364000000002</v>
       </c>
-      <c r="R7" s="20">
+      <c r="R7" s="19">
         <f>(U7+V7+W7)/0.95</f>
         <v>3.052631578947369</v>
       </c>
-      <c r="S7" s="16">
+      <c r="S7" s="15">
         <f>R7*Q7</f>
         <v>1.7706290063157899</v>
       </c>
-      <c r="T7" s="2">
+      <c r="T7" s="1">
         <v>500000000</v>
       </c>
       <c r="U7">
@@ -808,8 +865,32 @@
       <c r="W7">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X7" s="1">
+        <f>400000000/5*4</f>
+        <v>320000000</v>
+      </c>
+      <c r="Y7" s="27">
+        <f>L7/X7</f>
+        <v>0.90630256249999996</v>
+      </c>
+      <c r="Z7" s="27">
+        <f>R$8</f>
+        <v>2.4105263157894736</v>
+      </c>
+      <c r="AA7" s="27">
+        <f>Z7*Y7</f>
+        <v>2.1846661769736841</v>
+      </c>
+      <c r="AD7">
+        <f>AD$5*J7</f>
+        <v>40000</v>
+      </c>
+      <c r="AE7" s="30">
+        <f>AD7/T$8</f>
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0</v>
       </c>
@@ -835,41 +916,41 @@
         <f>B16</f>
         <v>16</v>
       </c>
-      <c r="K8" s="2">
+      <c r="K8" s="1">
         <f>C21</f>
         <v>27758525</v>
       </c>
-      <c r="L8" s="14">
+      <c r="L8" s="13">
         <f>K8*(J8+J7)</f>
         <v>555170500</v>
       </c>
-      <c r="M8" s="13">
+      <c r="M8" s="12">
         <f>2*K8</f>
         <v>55517050</v>
       </c>
-      <c r="N8" s="22">
+      <c r="N8" s="21">
         <v>4.2345499999999996</v>
       </c>
-      <c r="O8" s="7">
+      <c r="O8" s="6">
         <v>30.6</v>
       </c>
-      <c r="P8" s="18">
+      <c r="P8" s="17">
         <f t="shared" si="0"/>
         <v>129.57722999999999</v>
       </c>
-      <c r="Q8" s="22">
+      <c r="Q8" s="21">
         <f>L8/T8</f>
         <v>1.38792625</v>
       </c>
-      <c r="R8" s="20">
-        <f t="shared" ref="R8:R12" si="1">(U8+V8+W8)/0.95</f>
+      <c r="R8" s="19">
+        <f>(U8+V8+W8)/0.95</f>
         <v>2.4105263157894736</v>
       </c>
-      <c r="S8" s="16">
-        <f t="shared" ref="S8:S12" si="2">R8*Q8</f>
+      <c r="S8" s="15">
+        <f t="shared" ref="S8:S11" si="1">R8*Q8</f>
         <v>3.34563275</v>
       </c>
-      <c r="T8" s="2">
+      <c r="T8" s="1">
         <v>400000000</v>
       </c>
       <c r="U8">
@@ -881,8 +962,31 @@
       <c r="W8">
         <v>1.1000000000000001</v>
       </c>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X8" s="1">
+        <v>400000000</v>
+      </c>
+      <c r="Y8" s="27">
+        <f t="shared" ref="Y8:Y11" si="2">L8/X8</f>
+        <v>1.38792625</v>
+      </c>
+      <c r="Z8" s="27">
+        <f>R$8</f>
+        <v>2.4105263157894736</v>
+      </c>
+      <c r="AA8" s="27">
+        <f t="shared" ref="AA8:AA11" si="3">Z8*Y8</f>
+        <v>3.34563275</v>
+      </c>
+      <c r="AD8">
+        <f t="shared" ref="AD8:AD11" si="4">AD$5*J8</f>
+        <v>160000</v>
+      </c>
+      <c r="AE8" s="30">
+        <f t="shared" ref="AE8:AE11" si="5">AD8/T$8</f>
+        <v>4.0000000000000002E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0</v>
       </c>
@@ -908,41 +1012,41 @@
         <f>B23</f>
         <v>64</v>
       </c>
-      <c r="K9" s="15">
+      <c r="K9" s="14">
         <f>C27</f>
         <v>9189925</v>
       </c>
-      <c r="L9" s="14">
-        <f t="shared" ref="L9:L11" si="3">K9*(J9+J8)</f>
+      <c r="L9" s="13">
+        <f t="shared" ref="L9:L11" si="6">K9*(J9+J8)</f>
         <v>735194000</v>
       </c>
-      <c r="M9" s="13">
-        <f t="shared" ref="M9:M11" si="4">2*K9</f>
+      <c r="M9" s="12">
+        <f t="shared" ref="M9:M11" si="7">2*K9</f>
         <v>18379850</v>
       </c>
-      <c r="N9" s="22">
+      <c r="N9" s="21">
         <v>5.1720800000000002</v>
       </c>
-      <c r="O9" s="7">
+      <c r="O9" s="6">
         <v>30.6</v>
       </c>
-      <c r="P9" s="18">
+      <c r="P9" s="17">
         <f t="shared" si="0"/>
         <v>158.26564800000003</v>
       </c>
-      <c r="Q9" s="22">
-        <f t="shared" ref="Q8:Q11" si="5">L9/T9</f>
+      <c r="Q9" s="21">
+        <f t="shared" ref="Q9:Q11" si="8">L9/T9</f>
         <v>1.5221407867494825</v>
       </c>
-      <c r="R9" s="20">
+      <c r="R9" s="19">
+        <f t="shared" ref="R9:R12" si="9">(U9+V9+W9)/0.95</f>
+        <v>3.3789473684210529</v>
+      </c>
+      <c r="S9" s="15">
         <f t="shared" si="1"/>
-        <v>3.3789473684210529</v>
-      </c>
-      <c r="S9" s="16">
-        <f t="shared" si="2"/>
         <v>5.1432336057535153</v>
       </c>
-      <c r="T9" s="2">
+      <c r="T9" s="1">
         <v>483000000</v>
       </c>
       <c r="U9">
@@ -954,8 +1058,31 @@
       <c r="W9">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X9" s="1">
+        <v>400000000</v>
+      </c>
+      <c r="Y9" s="27">
+        <f t="shared" si="2"/>
+        <v>1.837985</v>
+      </c>
+      <c r="Z9" s="27">
+        <f>R$8</f>
+        <v>2.4105263157894736</v>
+      </c>
+      <c r="AA9" s="27">
+        <f t="shared" si="3"/>
+        <v>4.4305112105263156</v>
+      </c>
+      <c r="AD9">
+        <f t="shared" si="4"/>
+        <v>640000</v>
+      </c>
+      <c r="AE9" s="30">
+        <f t="shared" si="5"/>
+        <v>1.6000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0</v>
       </c>
@@ -981,41 +1108,41 @@
         <f>B29</f>
         <v>256</v>
       </c>
-      <c r="K10" s="15">
+      <c r="K10" s="14">
         <f>C32</f>
         <v>3227002</v>
       </c>
-      <c r="L10" s="13">
-        <f t="shared" si="3"/>
+      <c r="L10" s="12">
+        <f t="shared" si="6"/>
         <v>1032640640</v>
       </c>
-      <c r="M10" s="14">
-        <f t="shared" si="4"/>
+      <c r="M10" s="13">
+        <f t="shared" si="7"/>
         <v>6454004</v>
       </c>
-      <c r="N10" s="22">
+      <c r="N10" s="21">
         <v>6.9846500000000002</v>
       </c>
-      <c r="O10" s="7">
+      <c r="O10" s="6">
         <v>30.6</v>
       </c>
-      <c r="P10" s="18">
+      <c r="P10" s="17">
         <f t="shared" si="0"/>
         <v>213.73029000000002</v>
       </c>
-      <c r="Q10" s="22">
-        <f t="shared" si="5"/>
+      <c r="Q10" s="21">
+        <f t="shared" si="8"/>
         <v>2.0652812800000002</v>
       </c>
-      <c r="R10" s="20">
+      <c r="R10" s="19">
+        <f t="shared" si="9"/>
+        <v>2.9578947368421056</v>
+      </c>
+      <c r="S10" s="15">
         <f t="shared" si="1"/>
-        <v>2.9578947368421056</v>
-      </c>
-      <c r="S10" s="16">
-        <f t="shared" si="2"/>
         <v>6.1088846282105278</v>
       </c>
-      <c r="T10" s="2">
+      <c r="T10" s="1">
         <v>500000000</v>
       </c>
       <c r="U10">
@@ -1027,8 +1154,31 @@
       <c r="W10">
         <v>1.4</v>
       </c>
-    </row>
-    <row r="11" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="X10" s="1">
+        <v>400000000</v>
+      </c>
+      <c r="Y10" s="27">
+        <f t="shared" si="2"/>
+        <v>2.5816015999999999</v>
+      </c>
+      <c r="Z10" s="27">
+        <f>R$8</f>
+        <v>2.4105263157894736</v>
+      </c>
+      <c r="AA10" s="27">
+        <f t="shared" si="3"/>
+        <v>6.22301859368421</v>
+      </c>
+      <c r="AD10">
+        <f t="shared" si="4"/>
+        <v>2560000</v>
+      </c>
+      <c r="AE10" s="30">
+        <f t="shared" si="5"/>
+        <v>6.4000000000000003E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>0</v>
       </c>
@@ -1054,41 +1204,41 @@
         <f>B34</f>
         <v>1024</v>
       </c>
-      <c r="K11" s="15">
+      <c r="K11" s="14">
         <f>C36</f>
         <v>1182483</v>
       </c>
-      <c r="L11" s="13">
-        <f t="shared" si="3"/>
+      <c r="L11" s="12">
+        <f t="shared" si="6"/>
         <v>1513578240</v>
       </c>
-      <c r="M11" s="14">
-        <f t="shared" si="4"/>
+      <c r="M11" s="13">
+        <f t="shared" si="7"/>
         <v>2364966</v>
       </c>
-      <c r="N11" s="23">
+      <c r="N11" s="22">
         <v>10.6723</v>
       </c>
-      <c r="O11" s="9">
+      <c r="O11" s="8">
         <v>30.6</v>
       </c>
-      <c r="P11" s="19">
+      <c r="P11" s="18">
         <f>N11*O11</f>
         <v>326.57238000000001</v>
       </c>
-      <c r="Q11" s="23">
-        <f t="shared" si="5"/>
+      <c r="Q11" s="22">
+        <f t="shared" si="8"/>
         <v>3.0271564799999999</v>
       </c>
-      <c r="R11" s="21">
+      <c r="R11" s="20">
+        <f t="shared" si="9"/>
+        <v>2.8000000000000003</v>
+      </c>
+      <c r="S11" s="16">
         <f t="shared" si="1"/>
-        <v>2.8000000000000003</v>
-      </c>
-      <c r="S11" s="17">
-        <f t="shared" si="2"/>
         <v>8.4760381440000003</v>
       </c>
-      <c r="T11" s="2">
+      <c r="T11" s="1">
         <v>500000000</v>
       </c>
       <c r="U11">
@@ -1100,8 +1250,31 @@
       <c r="W11">
         <v>1.4</v>
       </c>
-    </row>
-    <row r="12" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="X11" s="1">
+        <v>400000000</v>
+      </c>
+      <c r="Y11" s="27">
+        <f t="shared" si="2"/>
+        <v>3.7839456</v>
+      </c>
+      <c r="Z11" s="27">
+        <f>R$8</f>
+        <v>2.4105263157894736</v>
+      </c>
+      <c r="AA11" s="27">
+        <f t="shared" si="3"/>
+        <v>9.1213004463157894</v>
+      </c>
+      <c r="AD11">
+        <f t="shared" si="4"/>
+        <v>10240000</v>
+      </c>
+      <c r="AE11" s="30">
+        <f t="shared" si="5"/>
+        <v>2.5600000000000001E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>0</v>
       </c>
@@ -1123,11 +1296,11 @@
       <c r="Q12">
         <v>0.25</v>
       </c>
-      <c r="R12" s="21">
-        <f t="shared" si="1"/>
+      <c r="R12" s="20">
+        <f t="shared" si="9"/>
         <v>1.8631578947368421</v>
       </c>
-      <c r="S12" s="17">
+      <c r="S12" s="16">
         <f>R12*Q12</f>
         <v>0.46578947368421053</v>
       </c>
@@ -1140,8 +1313,10 @@
       <c r="W12">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="13" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Y12" s="27"/>
+      <c r="AE12" s="30"/>
+    </row>
+    <row r="13" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C13">
         <f>SUM(C7:C12)</f>
         <v>72504205</v>
@@ -1149,47 +1324,70 @@
       <c r="I13" t="s">
         <v>17</v>
       </c>
-      <c r="N13" s="25">
+      <c r="N13" s="24">
         <f>SUM(N7:N11)</f>
         <v>29.923070000000003</v>
       </c>
-      <c r="O13" s="11">
+      <c r="O13" s="10">
         <f>P13/N13</f>
         <v>30.6</v>
       </c>
-      <c r="P13" s="26">
+      <c r="P13" s="25">
         <f>SUM(P7:P11)</f>
         <v>915.6459420000001</v>
       </c>
-      <c r="Q13" s="24">
+      <c r="Q13" s="23">
         <f>SUM(Q7:Q12)</f>
         <v>8.8325384367494824</v>
       </c>
-      <c r="R13" s="24">
+      <c r="R13" s="23">
         <f>S13/Q13</f>
         <v>2.865564388902746</v>
       </c>
-      <c r="S13" s="27">
+      <c r="S13" s="26">
         <f>SUM(S7:S12)</f>
         <v>25.310207607964045</v>
       </c>
-    </row>
-    <row r="14" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Y13" s="27">
+        <f>SUM(Y7:Y11)</f>
+        <v>10.4977610125</v>
+      </c>
+      <c r="Z13" s="27">
+        <f>AA13/Y13</f>
+        <v>2.4105263157894736</v>
+      </c>
+      <c r="AA13" s="27">
+        <f>SUM(AA7:AA11)</f>
+        <v>25.3051291775</v>
+      </c>
+      <c r="AE13" s="30">
+        <f>SUM(AE7:AE11)</f>
+        <v>3.4100000000000005E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I15" t="s">
         <v>18</v>
       </c>
-      <c r="Q15" s="10">
+      <c r="Q15" s="9">
         <f>N13/Q13</f>
         <v>3.3878222228277308</v>
       </c>
-      <c r="R15" s="11"/>
-      <c r="S15" s="12">
+      <c r="R15" s="10"/>
+      <c r="S15" s="11">
         <f>P13/S13</f>
         <v>36.176943159955954</v>
       </c>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y15" s="28">
+        <f>Y13/Q13-1</f>
+        <v>0.18853272903087936</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1494,9 +1692,10 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="N4:P4"/>
     <mergeCell ref="Q3:W3"/>
+    <mergeCell ref="X3:AA3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>